<commit_message>
added IDs to tooltips
</commit_message>
<xml_diff>
--- a/input/tooltips.xlsx
+++ b/input/tooltips.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="441">
   <si>
     <t>id</t>
   </si>
@@ -32,9 +32,6 @@
     <t>tooltip</t>
   </si>
   <si>
-    <t>Itt rövid leírás olvasható a kategóriáról</t>
-  </si>
-  <si>
     <t>K1</t>
   </si>
   <si>
@@ -342,6 +339,1014 @@
   </si>
   <si>
     <t>K513</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (1)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (2)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (3)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (4)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (5)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (6)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (7)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (8)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (9)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (10)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (12)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (13)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (14)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (15)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (16)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (17)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (18)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (19)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (20)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (21)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (22)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (24)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (25)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (26)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (27)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (28)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (29)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (30)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (31)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (32)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (33)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (34)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (35)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (36)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (37)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (38)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (39)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (40)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (41)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (42)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (43)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (44)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (45)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (46)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (47)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (48)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (49)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (50)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (52)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (53)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (54)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (58)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (59)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (60)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (62)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (65)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (67)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (68)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (69)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (70)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (71)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (72)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (73)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (74)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (79)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (80)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (83)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (84)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (89)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (93)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (94)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (95)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (97)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (98)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (109)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (111)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (113)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (114)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (115)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (116)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (117)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (118)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (121)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (123)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (124)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (133)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (144)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (146)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (160)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (167)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (168)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (176)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (177)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (179)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (180)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (184)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (186)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (187)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (188)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (189)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (190)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (191)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (192)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (193)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (195)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (196)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (197)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (198)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (200)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (201)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (202)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (206)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (209)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (218)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (219)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (221)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (222)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (227)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (231)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (235)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (237)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (239)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (245)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (253)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (257)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (261)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (264)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (265)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (283)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (286)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (287)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (294)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (296)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (298)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (299)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (305)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (307)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (310)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (316)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (412)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (421)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (451)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (471)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (474)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (510)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (520)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (540)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (610)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (630)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (640)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (660)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (721)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (722)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (723)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (740)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (810)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (820)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (840)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (860)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (911)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (912)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (921)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (960)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (1010)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (1011)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (1012)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (1013)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (1014)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (1021)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (1030)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (1040)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (1060)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (1070)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (9000)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (11130)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (13350)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (13370)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (16080)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (18010)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (18030)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (31030)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (41232)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (41233)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (41237)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (42120)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (45120)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (45160)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (47120)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (47410)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (51030)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (52020)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (52080)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (54010)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (61030)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (63080)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (64010)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (66010)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (66020)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (72111)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (72112)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (72210)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (72311)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (74011)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (74031)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (74032)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (81030)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (81041)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (81061)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (82042)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (82043)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (82044)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (82091)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (84031)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (84040)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (86010)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (86020)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (86030)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (86090)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (91140)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (91220)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (91250)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (92120)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (96015)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (101150)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (104042)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (104051)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (106020)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (107060)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (900020)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (K1)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (K11)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (K1101)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (K1104)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (K1107)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (K1109)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (K1110)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (K1113)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (K12)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (K121)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (K122)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (K123)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (K2)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (K3)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (K31)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (K311)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (K312)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (K32)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (K321)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (K322)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (K33)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (K331)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (K332)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (K333)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (K334)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (K335)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (K336)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (K337)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (K34)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (K341)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (K342)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (K35)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (K351)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (K352)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (K355)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (K4)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (K42)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (K47)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (K48)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (K5)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (K502)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (K5021)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (K512)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (K6)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (K62)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (K63)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (K64)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (K67)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (K7)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (K71)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (K73)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (K74)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (K8)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (K85)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (K9)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (K91)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (K914)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (K915)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (B1)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (B11)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (B111)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (B112)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (B113)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (B114)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (B115)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (B116)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (B16)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (B2)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (B21)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (B25)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (B3)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (B31)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (B311)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (B34)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (B35)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (B351)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (B354)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (B36)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (B4)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (B401)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (B402)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (B403)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (B404)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (B405)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (B406)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (B408)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (B4082)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (B410)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (B411)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (B5)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (B53)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (B6)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (B64)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (B65)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (B7)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (B74)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (B8)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (B81)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (B813)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (B8131)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (B814)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (K1103)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (K513)</t>
+  </si>
+  <si>
+    <t>FB</t>
+  </si>
+  <si>
+    <t>RE</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (FB)</t>
+  </si>
+  <si>
+    <t>Itt rövid leírás olvasható a kategóriáról (RE)</t>
   </si>
 </sst>
 </file>
@@ -660,9 +1665,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B333"/>
+  <dimension ref="A1:B335"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A307" workbookViewId="0">
+      <selection activeCell="A335" sqref="A335"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -679,7 +1686,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>105</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -687,7 +1694,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -695,7 +1702,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>2</v>
+        <v>107</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -703,7 +1710,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>2</v>
+        <v>108</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -711,7 +1718,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>2</v>
+        <v>109</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -719,7 +1726,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>2</v>
+        <v>110</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -727,7 +1734,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>2</v>
+        <v>111</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -735,7 +1742,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>2</v>
+        <v>112</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -743,7 +1750,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>2</v>
+        <v>113</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -751,7 +1758,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>2</v>
+        <v>114</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -759,7 +1766,7 @@
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>2</v>
+        <v>115</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -767,7 +1774,7 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>2</v>
+        <v>116</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -775,7 +1782,7 @@
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>2</v>
+        <v>117</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
@@ -783,7 +1790,7 @@
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>2</v>
+        <v>118</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
@@ -791,7 +1798,7 @@
         <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>2</v>
+        <v>119</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -799,7 +1806,7 @@
         <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>2</v>
+        <v>120</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
@@ -807,7 +1814,7 @@
         <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>2</v>
+        <v>121</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
@@ -815,7 +1822,7 @@
         <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>2</v>
+        <v>122</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
@@ -823,7 +1830,7 @@
         <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>2</v>
+        <v>123</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
@@ -831,7 +1838,7 @@
         <v>21</v>
       </c>
       <c r="B21" t="s">
-        <v>2</v>
+        <v>124</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
@@ -839,7 +1846,7 @@
         <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>2</v>
+        <v>125</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
@@ -847,7 +1854,7 @@
         <v>24</v>
       </c>
       <c r="B23" t="s">
-        <v>2</v>
+        <v>126</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
@@ -855,7 +1862,7 @@
         <v>25</v>
       </c>
       <c r="B24" t="s">
-        <v>2</v>
+        <v>127</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
@@ -863,7 +1870,7 @@
         <v>26</v>
       </c>
       <c r="B25" t="s">
-        <v>2</v>
+        <v>128</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
@@ -871,7 +1878,7 @@
         <v>27</v>
       </c>
       <c r="B26" t="s">
-        <v>2</v>
+        <v>129</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
@@ -879,7 +1886,7 @@
         <v>28</v>
       </c>
       <c r="B27" t="s">
-        <v>2</v>
+        <v>130</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
@@ -887,7 +1894,7 @@
         <v>29</v>
       </c>
       <c r="B28" t="s">
-        <v>2</v>
+        <v>131</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
@@ -895,7 +1902,7 @@
         <v>30</v>
       </c>
       <c r="B29" t="s">
-        <v>2</v>
+        <v>132</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
@@ -903,7 +1910,7 @@
         <v>31</v>
       </c>
       <c r="B30" t="s">
-        <v>2</v>
+        <v>133</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
@@ -911,7 +1918,7 @@
         <v>32</v>
       </c>
       <c r="B31" t="s">
-        <v>2</v>
+        <v>134</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
@@ -919,7 +1926,7 @@
         <v>33</v>
       </c>
       <c r="B32" t="s">
-        <v>2</v>
+        <v>135</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
@@ -927,7 +1934,7 @@
         <v>34</v>
       </c>
       <c r="B33" t="s">
-        <v>2</v>
+        <v>136</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
@@ -935,7 +1942,7 @@
         <v>35</v>
       </c>
       <c r="B34" t="s">
-        <v>2</v>
+        <v>137</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
@@ -943,7 +1950,7 @@
         <v>36</v>
       </c>
       <c r="B35" t="s">
-        <v>2</v>
+        <v>138</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
@@ -951,7 +1958,7 @@
         <v>37</v>
       </c>
       <c r="B36" t="s">
-        <v>2</v>
+        <v>139</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
@@ -959,7 +1966,7 @@
         <v>38</v>
       </c>
       <c r="B37" t="s">
-        <v>2</v>
+        <v>140</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
@@ -967,7 +1974,7 @@
         <v>39</v>
       </c>
       <c r="B38" t="s">
-        <v>2</v>
+        <v>141</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
@@ -975,7 +1982,7 @@
         <v>40</v>
       </c>
       <c r="B39" t="s">
-        <v>2</v>
+        <v>142</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
@@ -983,7 +1990,7 @@
         <v>41</v>
       </c>
       <c r="B40" t="s">
-        <v>2</v>
+        <v>143</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
@@ -991,7 +1998,7 @@
         <v>42</v>
       </c>
       <c r="B41" t="s">
-        <v>2</v>
+        <v>144</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
@@ -999,7 +2006,7 @@
         <v>43</v>
       </c>
       <c r="B42" t="s">
-        <v>2</v>
+        <v>145</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
@@ -1007,7 +2014,7 @@
         <v>44</v>
       </c>
       <c r="B43" t="s">
-        <v>2</v>
+        <v>146</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
@@ -1015,7 +2022,7 @@
         <v>45</v>
       </c>
       <c r="B44" t="s">
-        <v>2</v>
+        <v>147</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
@@ -1023,7 +2030,7 @@
         <v>46</v>
       </c>
       <c r="B45" t="s">
-        <v>2</v>
+        <v>148</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
@@ -1031,7 +2038,7 @@
         <v>47</v>
       </c>
       <c r="B46" t="s">
-        <v>2</v>
+        <v>149</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
@@ -1039,7 +2046,7 @@
         <v>48</v>
       </c>
       <c r="B47" t="s">
-        <v>2</v>
+        <v>150</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
@@ -1047,7 +2054,7 @@
         <v>49</v>
       </c>
       <c r="B48" t="s">
-        <v>2</v>
+        <v>151</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
@@ -1055,7 +2062,7 @@
         <v>50</v>
       </c>
       <c r="B49" t="s">
-        <v>2</v>
+        <v>152</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
@@ -1063,7 +2070,7 @@
         <v>52</v>
       </c>
       <c r="B50" t="s">
-        <v>2</v>
+        <v>153</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
@@ -1071,7 +2078,7 @@
         <v>53</v>
       </c>
       <c r="B51" t="s">
-        <v>2</v>
+        <v>154</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
@@ -1079,7 +2086,7 @@
         <v>54</v>
       </c>
       <c r="B52" t="s">
-        <v>2</v>
+        <v>155</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
@@ -1087,7 +2094,7 @@
         <v>58</v>
       </c>
       <c r="B53" t="s">
-        <v>2</v>
+        <v>156</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
@@ -1095,7 +2102,7 @@
         <v>59</v>
       </c>
       <c r="B54" t="s">
-        <v>2</v>
+        <v>157</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
@@ -1103,7 +2110,7 @@
         <v>60</v>
       </c>
       <c r="B55" t="s">
-        <v>2</v>
+        <v>158</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
@@ -1111,7 +2118,7 @@
         <v>62</v>
       </c>
       <c r="B56" t="s">
-        <v>2</v>
+        <v>159</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
@@ -1119,7 +2126,7 @@
         <v>65</v>
       </c>
       <c r="B57" t="s">
-        <v>2</v>
+        <v>160</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
@@ -1127,7 +2134,7 @@
         <v>67</v>
       </c>
       <c r="B58" t="s">
-        <v>2</v>
+        <v>161</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
@@ -1135,7 +2142,7 @@
         <v>68</v>
       </c>
       <c r="B59" t="s">
-        <v>2</v>
+        <v>162</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
@@ -1143,7 +2150,7 @@
         <v>69</v>
       </c>
       <c r="B60" t="s">
-        <v>2</v>
+        <v>163</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
@@ -1151,7 +2158,7 @@
         <v>70</v>
       </c>
       <c r="B61" t="s">
-        <v>2</v>
+        <v>164</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.3">
@@ -1159,7 +2166,7 @@
         <v>71</v>
       </c>
       <c r="B62" t="s">
-        <v>2</v>
+        <v>165</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.3">
@@ -1167,7 +2174,7 @@
         <v>72</v>
       </c>
       <c r="B63" t="s">
-        <v>2</v>
+        <v>166</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.3">
@@ -1175,7 +2182,7 @@
         <v>73</v>
       </c>
       <c r="B64" t="s">
-        <v>2</v>
+        <v>167</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
@@ -1183,7 +2190,7 @@
         <v>74</v>
       </c>
       <c r="B65" t="s">
-        <v>2</v>
+        <v>168</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
@@ -1191,7 +2198,7 @@
         <v>79</v>
       </c>
       <c r="B66" t="s">
-        <v>2</v>
+        <v>169</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.3">
@@ -1199,7 +2206,7 @@
         <v>80</v>
       </c>
       <c r="B67" t="s">
-        <v>2</v>
+        <v>170</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
@@ -1207,7 +2214,7 @@
         <v>83</v>
       </c>
       <c r="B68" t="s">
-        <v>2</v>
+        <v>171</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.3">
@@ -1215,7 +2222,7 @@
         <v>84</v>
       </c>
       <c r="B69" t="s">
-        <v>2</v>
+        <v>172</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
@@ -1223,7 +2230,7 @@
         <v>89</v>
       </c>
       <c r="B70" t="s">
-        <v>2</v>
+        <v>173</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.3">
@@ -1231,7 +2238,7 @@
         <v>93</v>
       </c>
       <c r="B71" t="s">
-        <v>2</v>
+        <v>174</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.3">
@@ -1239,7 +2246,7 @@
         <v>94</v>
       </c>
       <c r="B72" t="s">
-        <v>2</v>
+        <v>175</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.3">
@@ -1247,7 +2254,7 @@
         <v>95</v>
       </c>
       <c r="B73" t="s">
-        <v>2</v>
+        <v>176</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.3">
@@ -1255,7 +2262,7 @@
         <v>97</v>
       </c>
       <c r="B74" t="s">
-        <v>2</v>
+        <v>177</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.3">
@@ -1263,7 +2270,7 @@
         <v>98</v>
       </c>
       <c r="B75" t="s">
-        <v>2</v>
+        <v>178</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.3">
@@ -1271,7 +2278,7 @@
         <v>109</v>
       </c>
       <c r="B76" t="s">
-        <v>2</v>
+        <v>179</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.3">
@@ -1279,7 +2286,7 @@
         <v>111</v>
       </c>
       <c r="B77" t="s">
-        <v>2</v>
+        <v>180</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.3">
@@ -1287,7 +2294,7 @@
         <v>113</v>
       </c>
       <c r="B78" t="s">
-        <v>2</v>
+        <v>181</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.3">
@@ -1295,7 +2302,7 @@
         <v>114</v>
       </c>
       <c r="B79" t="s">
-        <v>2</v>
+        <v>182</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.3">
@@ -1303,7 +2310,7 @@
         <v>115</v>
       </c>
       <c r="B80" t="s">
-        <v>2</v>
+        <v>183</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.3">
@@ -1311,7 +2318,7 @@
         <v>116</v>
       </c>
       <c r="B81" t="s">
-        <v>2</v>
+        <v>184</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.3">
@@ -1319,7 +2326,7 @@
         <v>117</v>
       </c>
       <c r="B82" t="s">
-        <v>2</v>
+        <v>185</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.3">
@@ -1327,7 +2334,7 @@
         <v>118</v>
       </c>
       <c r="B83" t="s">
-        <v>2</v>
+        <v>186</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.3">
@@ -1335,7 +2342,7 @@
         <v>121</v>
       </c>
       <c r="B84" t="s">
-        <v>2</v>
+        <v>187</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.3">
@@ -1343,7 +2350,7 @@
         <v>123</v>
       </c>
       <c r="B85" t="s">
-        <v>2</v>
+        <v>188</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.3">
@@ -1351,7 +2358,7 @@
         <v>124</v>
       </c>
       <c r="B86" t="s">
-        <v>2</v>
+        <v>189</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.3">
@@ -1359,7 +2366,7 @@
         <v>133</v>
       </c>
       <c r="B87" t="s">
-        <v>2</v>
+        <v>190</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.3">
@@ -1367,7 +2374,7 @@
         <v>144</v>
       </c>
       <c r="B88" t="s">
-        <v>2</v>
+        <v>191</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.3">
@@ -1375,7 +2382,7 @@
         <v>146</v>
       </c>
       <c r="B89" t="s">
-        <v>2</v>
+        <v>192</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.3">
@@ -1383,7 +2390,7 @@
         <v>160</v>
       </c>
       <c r="B90" t="s">
-        <v>2</v>
+        <v>193</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.3">
@@ -1391,7 +2398,7 @@
         <v>167</v>
       </c>
       <c r="B91" t="s">
-        <v>2</v>
+        <v>194</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.3">
@@ -1399,7 +2406,7 @@
         <v>168</v>
       </c>
       <c r="B92" t="s">
-        <v>2</v>
+        <v>195</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.3">
@@ -1407,7 +2414,7 @@
         <v>176</v>
       </c>
       <c r="B93" t="s">
-        <v>2</v>
+        <v>196</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.3">
@@ -1415,7 +2422,7 @@
         <v>177</v>
       </c>
       <c r="B94" t="s">
-        <v>2</v>
+        <v>197</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.3">
@@ -1423,7 +2430,7 @@
         <v>179</v>
       </c>
       <c r="B95" t="s">
-        <v>2</v>
+        <v>198</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.3">
@@ -1431,7 +2438,7 @@
         <v>180</v>
       </c>
       <c r="B96" t="s">
-        <v>2</v>
+        <v>199</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.3">
@@ -1439,7 +2446,7 @@
         <v>184</v>
       </c>
       <c r="B97" t="s">
-        <v>2</v>
+        <v>200</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.3">
@@ -1447,7 +2454,7 @@
         <v>186</v>
       </c>
       <c r="B98" t="s">
-        <v>2</v>
+        <v>201</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.3">
@@ -1455,7 +2462,7 @@
         <v>187</v>
       </c>
       <c r="B99" t="s">
-        <v>2</v>
+        <v>202</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.3">
@@ -1463,7 +2470,7 @@
         <v>188</v>
       </c>
       <c r="B100" t="s">
-        <v>2</v>
+        <v>203</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.3">
@@ -1471,7 +2478,7 @@
         <v>189</v>
       </c>
       <c r="B101" t="s">
-        <v>2</v>
+        <v>204</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.3">
@@ -1479,7 +2486,7 @@
         <v>190</v>
       </c>
       <c r="B102" t="s">
-        <v>2</v>
+        <v>205</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.3">
@@ -1487,7 +2494,7 @@
         <v>191</v>
       </c>
       <c r="B103" t="s">
-        <v>2</v>
+        <v>206</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.3">
@@ -1495,7 +2502,7 @@
         <v>192</v>
       </c>
       <c r="B104" t="s">
-        <v>2</v>
+        <v>207</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.3">
@@ -1503,7 +2510,7 @@
         <v>193</v>
       </c>
       <c r="B105" t="s">
-        <v>2</v>
+        <v>208</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.3">
@@ -1511,7 +2518,7 @@
         <v>195</v>
       </c>
       <c r="B106" t="s">
-        <v>2</v>
+        <v>209</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.3">
@@ -1519,7 +2526,7 @@
         <v>196</v>
       </c>
       <c r="B107" t="s">
-        <v>2</v>
+        <v>210</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.3">
@@ -1527,7 +2534,7 @@
         <v>197</v>
       </c>
       <c r="B108" t="s">
-        <v>2</v>
+        <v>211</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.3">
@@ -1535,7 +2542,7 @@
         <v>198</v>
       </c>
       <c r="B109" t="s">
-        <v>2</v>
+        <v>212</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.3">
@@ -1543,7 +2550,7 @@
         <v>200</v>
       </c>
       <c r="B110" t="s">
-        <v>2</v>
+        <v>213</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.3">
@@ -1551,7 +2558,7 @@
         <v>201</v>
       </c>
       <c r="B111" t="s">
-        <v>2</v>
+        <v>214</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.3">
@@ -1559,7 +2566,7 @@
         <v>202</v>
       </c>
       <c r="B112" t="s">
-        <v>2</v>
+        <v>215</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.3">
@@ -1567,7 +2574,7 @@
         <v>206</v>
       </c>
       <c r="B113" t="s">
-        <v>2</v>
+        <v>216</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.3">
@@ -1575,7 +2582,7 @@
         <v>209</v>
       </c>
       <c r="B114" t="s">
-        <v>2</v>
+        <v>217</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.3">
@@ -1583,7 +2590,7 @@
         <v>218</v>
       </c>
       <c r="B115" t="s">
-        <v>2</v>
+        <v>218</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.3">
@@ -1591,7 +2598,7 @@
         <v>219</v>
       </c>
       <c r="B116" t="s">
-        <v>2</v>
+        <v>219</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.3">
@@ -1599,7 +2606,7 @@
         <v>221</v>
       </c>
       <c r="B117" t="s">
-        <v>2</v>
+        <v>220</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.3">
@@ -1607,7 +2614,7 @@
         <v>222</v>
       </c>
       <c r="B118" t="s">
-        <v>2</v>
+        <v>221</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.3">
@@ -1615,7 +2622,7 @@
         <v>227</v>
       </c>
       <c r="B119" t="s">
-        <v>2</v>
+        <v>222</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.3">
@@ -1623,7 +2630,7 @@
         <v>231</v>
       </c>
       <c r="B120" t="s">
-        <v>2</v>
+        <v>223</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.3">
@@ -1631,7 +2638,7 @@
         <v>235</v>
       </c>
       <c r="B121" t="s">
-        <v>2</v>
+        <v>224</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.3">
@@ -1639,7 +2646,7 @@
         <v>237</v>
       </c>
       <c r="B122" t="s">
-        <v>2</v>
+        <v>225</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.3">
@@ -1647,7 +2654,7 @@
         <v>239</v>
       </c>
       <c r="B123" t="s">
-        <v>2</v>
+        <v>226</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.3">
@@ -1655,7 +2662,7 @@
         <v>245</v>
       </c>
       <c r="B124" t="s">
-        <v>2</v>
+        <v>227</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.3">
@@ -1663,7 +2670,7 @@
         <v>253</v>
       </c>
       <c r="B125" t="s">
-        <v>2</v>
+        <v>228</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.3">
@@ -1671,7 +2678,7 @@
         <v>257</v>
       </c>
       <c r="B126" t="s">
-        <v>2</v>
+        <v>229</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.3">
@@ -1679,7 +2686,7 @@
         <v>261</v>
       </c>
       <c r="B127" t="s">
-        <v>2</v>
+        <v>230</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.3">
@@ -1687,7 +2694,7 @@
         <v>264</v>
       </c>
       <c r="B128" t="s">
-        <v>2</v>
+        <v>231</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.3">
@@ -1695,7 +2702,7 @@
         <v>265</v>
       </c>
       <c r="B129" t="s">
-        <v>2</v>
+        <v>232</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.3">
@@ -1703,7 +2710,7 @@
         <v>283</v>
       </c>
       <c r="B130" t="s">
-        <v>2</v>
+        <v>233</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.3">
@@ -1711,7 +2718,7 @@
         <v>286</v>
       </c>
       <c r="B131" t="s">
-        <v>2</v>
+        <v>234</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.3">
@@ -1719,7 +2726,7 @@
         <v>287</v>
       </c>
       <c r="B132" t="s">
-        <v>2</v>
+        <v>235</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.3">
@@ -1727,7 +2734,7 @@
         <v>294</v>
       </c>
       <c r="B133" t="s">
-        <v>2</v>
+        <v>236</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.3">
@@ -1735,7 +2742,7 @@
         <v>296</v>
       </c>
       <c r="B134" t="s">
-        <v>2</v>
+        <v>237</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.3">
@@ -1743,7 +2750,7 @@
         <v>298</v>
       </c>
       <c r="B135" t="s">
-        <v>2</v>
+        <v>238</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.3">
@@ -1751,7 +2758,7 @@
         <v>299</v>
       </c>
       <c r="B136" t="s">
-        <v>2</v>
+        <v>239</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.3">
@@ -1759,7 +2766,7 @@
         <v>305</v>
       </c>
       <c r="B137" t="s">
-        <v>2</v>
+        <v>240</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.3">
@@ -1767,7 +2774,7 @@
         <v>307</v>
       </c>
       <c r="B138" t="s">
-        <v>2</v>
+        <v>241</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.3">
@@ -1775,7 +2782,7 @@
         <v>310</v>
       </c>
       <c r="B139" t="s">
-        <v>2</v>
+        <v>242</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.3">
@@ -1783,7 +2790,7 @@
         <v>316</v>
       </c>
       <c r="B140" t="s">
-        <v>2</v>
+        <v>243</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.3">
@@ -1791,7 +2798,7 @@
         <v>412</v>
       </c>
       <c r="B141" t="s">
-        <v>2</v>
+        <v>244</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.3">
@@ -1799,7 +2806,7 @@
         <v>421</v>
       </c>
       <c r="B142" t="s">
-        <v>2</v>
+        <v>245</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.3">
@@ -1807,7 +2814,7 @@
         <v>451</v>
       </c>
       <c r="B143" t="s">
-        <v>2</v>
+        <v>246</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.3">
@@ -1815,7 +2822,7 @@
         <v>471</v>
       </c>
       <c r="B144" t="s">
-        <v>2</v>
+        <v>247</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.3">
@@ -1823,7 +2830,7 @@
         <v>474</v>
       </c>
       <c r="B145" t="s">
-        <v>2</v>
+        <v>248</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.3">
@@ -1831,7 +2838,7 @@
         <v>510</v>
       </c>
       <c r="B146" t="s">
-        <v>2</v>
+        <v>249</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.3">
@@ -1839,7 +2846,7 @@
         <v>520</v>
       </c>
       <c r="B147" t="s">
-        <v>2</v>
+        <v>250</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.3">
@@ -1847,7 +2854,7 @@
         <v>540</v>
       </c>
       <c r="B148" t="s">
-        <v>2</v>
+        <v>251</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.3">
@@ -1855,7 +2862,7 @@
         <v>610</v>
       </c>
       <c r="B149" t="s">
-        <v>2</v>
+        <v>252</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.3">
@@ -1863,7 +2870,7 @@
         <v>630</v>
       </c>
       <c r="B150" t="s">
-        <v>2</v>
+        <v>253</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.3">
@@ -1871,7 +2878,7 @@
         <v>640</v>
       </c>
       <c r="B151" t="s">
-        <v>2</v>
+        <v>254</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.3">
@@ -1879,7 +2886,7 @@
         <v>660</v>
       </c>
       <c r="B152" t="s">
-        <v>2</v>
+        <v>255</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.3">
@@ -1887,7 +2894,7 @@
         <v>721</v>
       </c>
       <c r="B153" t="s">
-        <v>2</v>
+        <v>256</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.3">
@@ -1895,7 +2902,7 @@
         <v>722</v>
       </c>
       <c r="B154" t="s">
-        <v>2</v>
+        <v>257</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.3">
@@ -1903,7 +2910,7 @@
         <v>723</v>
       </c>
       <c r="B155" t="s">
-        <v>2</v>
+        <v>258</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.3">
@@ -1911,7 +2918,7 @@
         <v>740</v>
       </c>
       <c r="B156" t="s">
-        <v>2</v>
+        <v>259</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.3">
@@ -1919,7 +2926,7 @@
         <v>810</v>
       </c>
       <c r="B157" t="s">
-        <v>2</v>
+        <v>260</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.3">
@@ -1927,7 +2934,7 @@
         <v>820</v>
       </c>
       <c r="B158" t="s">
-        <v>2</v>
+        <v>261</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.3">
@@ -1935,7 +2942,7 @@
         <v>840</v>
       </c>
       <c r="B159" t="s">
-        <v>2</v>
+        <v>262</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.3">
@@ -1943,7 +2950,7 @@
         <v>860</v>
       </c>
       <c r="B160" t="s">
-        <v>2</v>
+        <v>263</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.3">
@@ -1951,7 +2958,7 @@
         <v>911</v>
       </c>
       <c r="B161" t="s">
-        <v>2</v>
+        <v>264</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.3">
@@ -1959,7 +2966,7 @@
         <v>912</v>
       </c>
       <c r="B162" t="s">
-        <v>2</v>
+        <v>265</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.3">
@@ -1967,7 +2974,7 @@
         <v>921</v>
       </c>
       <c r="B163" t="s">
-        <v>2</v>
+        <v>266</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.3">
@@ -1975,7 +2982,7 @@
         <v>960</v>
       </c>
       <c r="B164" t="s">
-        <v>2</v>
+        <v>267</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.3">
@@ -1983,7 +2990,7 @@
         <v>1010</v>
       </c>
       <c r="B165" t="s">
-        <v>2</v>
+        <v>268</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.3">
@@ -1991,7 +2998,7 @@
         <v>1011</v>
       </c>
       <c r="B166" t="s">
-        <v>2</v>
+        <v>269</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.3">
@@ -1999,7 +3006,7 @@
         <v>1012</v>
       </c>
       <c r="B167" t="s">
-        <v>2</v>
+        <v>270</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.3">
@@ -2007,7 +3014,7 @@
         <v>1013</v>
       </c>
       <c r="B168" t="s">
-        <v>2</v>
+        <v>271</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.3">
@@ -2015,7 +3022,7 @@
         <v>1014</v>
       </c>
       <c r="B169" t="s">
-        <v>2</v>
+        <v>272</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.3">
@@ -2023,7 +3030,7 @@
         <v>1021</v>
       </c>
       <c r="B170" t="s">
-        <v>2</v>
+        <v>273</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.3">
@@ -2031,7 +3038,7 @@
         <v>1030</v>
       </c>
       <c r="B171" t="s">
-        <v>2</v>
+        <v>274</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.3">
@@ -2039,7 +3046,7 @@
         <v>1040</v>
       </c>
       <c r="B172" t="s">
-        <v>2</v>
+        <v>275</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.3">
@@ -2047,7 +3054,7 @@
         <v>1060</v>
       </c>
       <c r="B173" t="s">
-        <v>2</v>
+        <v>276</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.3">
@@ -2055,7 +3062,7 @@
         <v>1070</v>
       </c>
       <c r="B174" t="s">
-        <v>2</v>
+        <v>277</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.3">
@@ -2063,7 +3070,7 @@
         <v>9000</v>
       </c>
       <c r="B175" t="s">
-        <v>2</v>
+        <v>278</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.3">
@@ -2071,7 +3078,7 @@
         <v>11130</v>
       </c>
       <c r="B176" t="s">
-        <v>2</v>
+        <v>279</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.3">
@@ -2079,7 +3086,7 @@
         <v>13350</v>
       </c>
       <c r="B177" t="s">
-        <v>2</v>
+        <v>280</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.3">
@@ -2087,7 +3094,7 @@
         <v>13370</v>
       </c>
       <c r="B178" t="s">
-        <v>2</v>
+        <v>281</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.3">
@@ -2095,7 +3102,7 @@
         <v>16080</v>
       </c>
       <c r="B179" t="s">
-        <v>2</v>
+        <v>282</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.3">
@@ -2103,7 +3110,7 @@
         <v>18010</v>
       </c>
       <c r="B180" t="s">
-        <v>2</v>
+        <v>283</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.3">
@@ -2111,7 +3118,7 @@
         <v>18030</v>
       </c>
       <c r="B181" t="s">
-        <v>2</v>
+        <v>284</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.3">
@@ -2119,7 +3126,7 @@
         <v>31030</v>
       </c>
       <c r="B182" t="s">
-        <v>2</v>
+        <v>285</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.3">
@@ -2127,7 +3134,7 @@
         <v>41232</v>
       </c>
       <c r="B183" t="s">
-        <v>2</v>
+        <v>286</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.3">
@@ -2135,7 +3142,7 @@
         <v>41233</v>
       </c>
       <c r="B184" t="s">
-        <v>2</v>
+        <v>287</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.3">
@@ -2143,7 +3150,7 @@
         <v>41237</v>
       </c>
       <c r="B185" t="s">
-        <v>2</v>
+        <v>288</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.3">
@@ -2151,7 +3158,7 @@
         <v>42120</v>
       </c>
       <c r="B186" t="s">
-        <v>2</v>
+        <v>289</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.3">
@@ -2159,7 +3166,7 @@
         <v>45120</v>
       </c>
       <c r="B187" t="s">
-        <v>2</v>
+        <v>290</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.3">
@@ -2167,7 +3174,7 @@
         <v>45160</v>
       </c>
       <c r="B188" t="s">
-        <v>2</v>
+        <v>291</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.3">
@@ -2175,7 +3182,7 @@
         <v>47120</v>
       </c>
       <c r="B189" t="s">
-        <v>2</v>
+        <v>292</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.3">
@@ -2183,7 +3190,7 @@
         <v>47410</v>
       </c>
       <c r="B190" t="s">
-        <v>2</v>
+        <v>293</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.3">
@@ -2191,7 +3198,7 @@
         <v>51030</v>
       </c>
       <c r="B191" t="s">
-        <v>2</v>
+        <v>294</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.3">
@@ -2199,7 +3206,7 @@
         <v>52020</v>
       </c>
       <c r="B192" t="s">
-        <v>2</v>
+        <v>295</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.3">
@@ -2207,7 +3214,7 @@
         <v>52080</v>
       </c>
       <c r="B193" t="s">
-        <v>2</v>
+        <v>296</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.3">
@@ -2215,7 +3222,7 @@
         <v>54010</v>
       </c>
       <c r="B194" t="s">
-        <v>2</v>
+        <v>297</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.3">
@@ -2223,7 +3230,7 @@
         <v>61030</v>
       </c>
       <c r="B195" t="s">
-        <v>2</v>
+        <v>298</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.3">
@@ -2231,7 +3238,7 @@
         <v>63080</v>
       </c>
       <c r="B196" t="s">
-        <v>2</v>
+        <v>299</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.3">
@@ -2239,7 +3246,7 @@
         <v>64010</v>
       </c>
       <c r="B197" t="s">
-        <v>2</v>
+        <v>300</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.3">
@@ -2247,7 +3254,7 @@
         <v>66010</v>
       </c>
       <c r="B198" t="s">
-        <v>2</v>
+        <v>301</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.3">
@@ -2255,7 +3262,7 @@
         <v>66020</v>
       </c>
       <c r="B199" t="s">
-        <v>2</v>
+        <v>302</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.3">
@@ -2263,7 +3270,7 @@
         <v>72111</v>
       </c>
       <c r="B200" t="s">
-        <v>2</v>
+        <v>303</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.3">
@@ -2271,7 +3278,7 @@
         <v>72112</v>
       </c>
       <c r="B201" t="s">
-        <v>2</v>
+        <v>304</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.3">
@@ -2279,7 +3286,7 @@
         <v>72210</v>
       </c>
       <c r="B202" t="s">
-        <v>2</v>
+        <v>305</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.3">
@@ -2287,7 +3294,7 @@
         <v>72311</v>
       </c>
       <c r="B203" t="s">
-        <v>2</v>
+        <v>306</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.3">
@@ -2295,7 +3302,7 @@
         <v>74011</v>
       </c>
       <c r="B204" t="s">
-        <v>2</v>
+        <v>307</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.3">
@@ -2303,7 +3310,7 @@
         <v>74031</v>
       </c>
       <c r="B205" t="s">
-        <v>2</v>
+        <v>308</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.3">
@@ -2311,7 +3318,7 @@
         <v>74032</v>
       </c>
       <c r="B206" t="s">
-        <v>2</v>
+        <v>309</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.3">
@@ -2319,7 +3326,7 @@
         <v>81030</v>
       </c>
       <c r="B207" t="s">
-        <v>2</v>
+        <v>310</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.3">
@@ -2327,7 +3334,7 @@
         <v>81041</v>
       </c>
       <c r="B208" t="s">
-        <v>2</v>
+        <v>311</v>
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.3">
@@ -2335,7 +3342,7 @@
         <v>81061</v>
       </c>
       <c r="B209" t="s">
-        <v>2</v>
+        <v>312</v>
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.3">
@@ -2343,7 +3350,7 @@
         <v>82042</v>
       </c>
       <c r="B210" t="s">
-        <v>2</v>
+        <v>313</v>
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.3">
@@ -2351,7 +3358,7 @@
         <v>82043</v>
       </c>
       <c r="B211" t="s">
-        <v>2</v>
+        <v>314</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.3">
@@ -2359,7 +3366,7 @@
         <v>82044</v>
       </c>
       <c r="B212" t="s">
-        <v>2</v>
+        <v>315</v>
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.3">
@@ -2367,7 +3374,7 @@
         <v>82091</v>
       </c>
       <c r="B213" t="s">
-        <v>2</v>
+        <v>316</v>
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.3">
@@ -2375,7 +3382,7 @@
         <v>84031</v>
       </c>
       <c r="B214" t="s">
-        <v>2</v>
+        <v>317</v>
       </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.3">
@@ -2383,7 +3390,7 @@
         <v>84040</v>
       </c>
       <c r="B215" t="s">
-        <v>2</v>
+        <v>318</v>
       </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.3">
@@ -2391,7 +3398,7 @@
         <v>86010</v>
       </c>
       <c r="B216" t="s">
-        <v>2</v>
+        <v>319</v>
       </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.3">
@@ -2399,7 +3406,7 @@
         <v>86020</v>
       </c>
       <c r="B217" t="s">
-        <v>2</v>
+        <v>320</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.3">
@@ -2407,7 +3414,7 @@
         <v>86030</v>
       </c>
       <c r="B218" t="s">
-        <v>2</v>
+        <v>321</v>
       </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.3">
@@ -2415,7 +3422,7 @@
         <v>86090</v>
       </c>
       <c r="B219" t="s">
-        <v>2</v>
+        <v>322</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.3">
@@ -2423,7 +3430,7 @@
         <v>91140</v>
       </c>
       <c r="B220" t="s">
-        <v>2</v>
+        <v>323</v>
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.3">
@@ -2431,7 +3438,7 @@
         <v>91220</v>
       </c>
       <c r="B221" t="s">
-        <v>2</v>
+        <v>324</v>
       </c>
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.3">
@@ -2439,7 +3446,7 @@
         <v>91250</v>
       </c>
       <c r="B222" t="s">
-        <v>2</v>
+        <v>325</v>
       </c>
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.3">
@@ -2447,7 +3454,7 @@
         <v>92120</v>
       </c>
       <c r="B223" t="s">
-        <v>2</v>
+        <v>326</v>
       </c>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.3">
@@ -2455,7 +3462,7 @@
         <v>96015</v>
       </c>
       <c r="B224" t="s">
-        <v>2</v>
+        <v>327</v>
       </c>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.3">
@@ -2463,7 +3470,7 @@
         <v>101150</v>
       </c>
       <c r="B225" t="s">
-        <v>2</v>
+        <v>328</v>
       </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.3">
@@ -2471,7 +3478,7 @@
         <v>104042</v>
       </c>
       <c r="B226" t="s">
-        <v>2</v>
+        <v>329</v>
       </c>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.3">
@@ -2479,7 +3486,7 @@
         <v>104051</v>
       </c>
       <c r="B227" t="s">
-        <v>2</v>
+        <v>330</v>
       </c>
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.3">
@@ -2487,7 +3494,7 @@
         <v>106020</v>
       </c>
       <c r="B228" t="s">
-        <v>2</v>
+        <v>331</v>
       </c>
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.3">
@@ -2495,7 +3502,7 @@
         <v>107060</v>
       </c>
       <c r="B229" t="s">
-        <v>2</v>
+        <v>332</v>
       </c>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.3">
@@ -2503,831 +3510,847 @@
         <v>900020</v>
       </c>
       <c r="B230" t="s">
-        <v>2</v>
+        <v>333</v>
       </c>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B231" t="s">
-        <v>2</v>
+        <v>334</v>
       </c>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B232" t="s">
-        <v>2</v>
+        <v>335</v>
       </c>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B233" t="s">
-        <v>2</v>
+        <v>336</v>
       </c>
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B234" t="s">
-        <v>2</v>
+        <v>337</v>
       </c>
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B235" t="s">
-        <v>2</v>
+        <v>338</v>
       </c>
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B236" t="s">
-        <v>2</v>
+        <v>339</v>
       </c>
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B237" t="s">
-        <v>2</v>
+        <v>340</v>
       </c>
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B238" t="s">
-        <v>2</v>
+        <v>341</v>
       </c>
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B239" t="s">
-        <v>2</v>
+        <v>342</v>
       </c>
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B240" t="s">
-        <v>2</v>
+        <v>343</v>
       </c>
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B241" t="s">
-        <v>2</v>
+        <v>344</v>
       </c>
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B242" t="s">
-        <v>2</v>
+        <v>345</v>
       </c>
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A243" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B243" t="s">
-        <v>2</v>
+        <v>346</v>
       </c>
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B244" t="s">
-        <v>2</v>
+        <v>347</v>
       </c>
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B245" t="s">
-        <v>2</v>
+        <v>348</v>
       </c>
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B246" t="s">
-        <v>2</v>
+        <v>349</v>
       </c>
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B247" t="s">
-        <v>2</v>
+        <v>350</v>
       </c>
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A248" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B248" t="s">
-        <v>2</v>
+        <v>351</v>
       </c>
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B249" t="s">
-        <v>2</v>
+        <v>352</v>
       </c>
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A250" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B250" t="s">
-        <v>2</v>
+        <v>353</v>
       </c>
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A251" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B251" t="s">
-        <v>2</v>
+        <v>354</v>
       </c>
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A252" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B252" t="s">
-        <v>2</v>
+        <v>355</v>
       </c>
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A253" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B253" t="s">
-        <v>2</v>
+        <v>356</v>
       </c>
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B254" t="s">
-        <v>2</v>
+        <v>357</v>
       </c>
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A255" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B255" t="s">
-        <v>2</v>
+        <v>358</v>
       </c>
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B256" t="s">
-        <v>2</v>
+        <v>359</v>
       </c>
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A257" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B257" t="s">
-        <v>2</v>
+        <v>360</v>
       </c>
     </row>
     <row r="258" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A258" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B258" t="s">
-        <v>2</v>
+        <v>361</v>
       </c>
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A259" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B259" t="s">
-        <v>2</v>
+        <v>362</v>
       </c>
     </row>
     <row r="260" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A260" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B260" t="s">
-        <v>2</v>
+        <v>363</v>
       </c>
     </row>
     <row r="261" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A261" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B261" t="s">
-        <v>2</v>
+        <v>364</v>
       </c>
     </row>
     <row r="262" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A262" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B262" t="s">
-        <v>2</v>
+        <v>365</v>
       </c>
     </row>
     <row r="263" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A263" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B263" t="s">
-        <v>2</v>
+        <v>366</v>
       </c>
     </row>
     <row r="264" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A264" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B264" t="s">
-        <v>2</v>
+        <v>367</v>
       </c>
     </row>
     <row r="265" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A265" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B265" t="s">
-        <v>2</v>
+        <v>368</v>
       </c>
     </row>
     <row r="266" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A266" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B266" t="s">
-        <v>2</v>
+        <v>369</v>
       </c>
     </row>
     <row r="267" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A267" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B267" t="s">
-        <v>2</v>
+        <v>370</v>
       </c>
     </row>
     <row r="268" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A268" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B268" t="s">
-        <v>2</v>
+        <v>371</v>
       </c>
     </row>
     <row r="269" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A269" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B269" t="s">
-        <v>2</v>
+        <v>372</v>
       </c>
     </row>
     <row r="270" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A270" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B270" t="s">
-        <v>2</v>
+        <v>373</v>
       </c>
     </row>
     <row r="271" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A271" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B271" t="s">
-        <v>2</v>
+        <v>374</v>
       </c>
     </row>
     <row r="272" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A272" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B272" t="s">
-        <v>2</v>
+        <v>375</v>
       </c>
     </row>
     <row r="273" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A273" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B273" t="s">
-        <v>2</v>
+        <v>376</v>
       </c>
     </row>
     <row r="274" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A274" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B274" t="s">
-        <v>2</v>
+        <v>377</v>
       </c>
     </row>
     <row r="275" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A275" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B275" t="s">
-        <v>2</v>
+        <v>378</v>
       </c>
     </row>
     <row r="276" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A276" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B276" t="s">
-        <v>2</v>
+        <v>379</v>
       </c>
     </row>
     <row r="277" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A277" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B277" t="s">
-        <v>2</v>
+        <v>380</v>
       </c>
     </row>
     <row r="278" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A278" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B278" t="s">
-        <v>2</v>
+        <v>381</v>
       </c>
     </row>
     <row r="279" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A279" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B279" t="s">
-        <v>2</v>
+        <v>382</v>
       </c>
     </row>
     <row r="280" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A280" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B280" t="s">
-        <v>2</v>
+        <v>383</v>
       </c>
     </row>
     <row r="281" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A281" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B281" t="s">
-        <v>2</v>
+        <v>384</v>
       </c>
     </row>
     <row r="282" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A282" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B282" t="s">
-        <v>2</v>
+        <v>385</v>
       </c>
     </row>
     <row r="283" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A283" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B283" t="s">
-        <v>2</v>
+        <v>386</v>
       </c>
     </row>
     <row r="284" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A284" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B284" t="s">
-        <v>2</v>
+        <v>387</v>
       </c>
     </row>
     <row r="285" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A285" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B285" t="s">
-        <v>2</v>
+        <v>388</v>
       </c>
     </row>
     <row r="286" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A286" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B286" t="s">
-        <v>2</v>
+        <v>389</v>
       </c>
     </row>
     <row r="287" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A287" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B287" t="s">
-        <v>2</v>
+        <v>390</v>
       </c>
     </row>
     <row r="288" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A288" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B288" t="s">
-        <v>2</v>
+        <v>391</v>
       </c>
     </row>
     <row r="289" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A289" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B289" t="s">
-        <v>2</v>
+        <v>392</v>
       </c>
     </row>
     <row r="290" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A290" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B290" t="s">
-        <v>2</v>
+        <v>393</v>
       </c>
     </row>
     <row r="291" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A291" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B291" t="s">
-        <v>2</v>
+        <v>394</v>
       </c>
     </row>
     <row r="292" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A292" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B292" t="s">
-        <v>2</v>
+        <v>395</v>
       </c>
     </row>
     <row r="293" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A293" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B293" t="s">
-        <v>2</v>
+        <v>396</v>
       </c>
     </row>
     <row r="294" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A294" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B294" t="s">
-        <v>2</v>
+        <v>397</v>
       </c>
     </row>
     <row r="295" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A295" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B295" t="s">
-        <v>2</v>
+        <v>398</v>
       </c>
     </row>
     <row r="296" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A296" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B296" t="s">
-        <v>2</v>
+        <v>399</v>
       </c>
     </row>
     <row r="297" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A297" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B297" t="s">
-        <v>2</v>
+        <v>400</v>
       </c>
     </row>
     <row r="298" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A298" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B298" t="s">
-        <v>2</v>
+        <v>401</v>
       </c>
     </row>
     <row r="299" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A299" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B299" t="s">
-        <v>2</v>
+        <v>402</v>
       </c>
     </row>
     <row r="300" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A300" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B300" t="s">
-        <v>2</v>
+        <v>403</v>
       </c>
     </row>
     <row r="301" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A301" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B301" t="s">
-        <v>2</v>
+        <v>404</v>
       </c>
     </row>
     <row r="302" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A302" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B302" t="s">
-        <v>2</v>
+        <v>405</v>
       </c>
     </row>
     <row r="303" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A303" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B303" t="s">
-        <v>2</v>
+        <v>406</v>
       </c>
     </row>
     <row r="304" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A304" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B304" t="s">
-        <v>2</v>
+        <v>407</v>
       </c>
     </row>
     <row r="305" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A305" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B305" t="s">
-        <v>2</v>
+        <v>408</v>
       </c>
     </row>
     <row r="306" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A306" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B306" t="s">
-        <v>2</v>
+        <v>409</v>
       </c>
     </row>
     <row r="307" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A307" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B307" t="s">
-        <v>2</v>
+        <v>410</v>
       </c>
     </row>
     <row r="308" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A308" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B308" t="s">
-        <v>2</v>
+        <v>411</v>
       </c>
     </row>
     <row r="309" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A309" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B309" t="s">
-        <v>2</v>
+        <v>412</v>
       </c>
     </row>
     <row r="310" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A310" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B310" t="s">
-        <v>2</v>
+        <v>413</v>
       </c>
     </row>
     <row r="311" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A311" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B311" t="s">
-        <v>2</v>
+        <v>414</v>
       </c>
     </row>
     <row r="312" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A312" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B312" t="s">
-        <v>2</v>
+        <v>415</v>
       </c>
     </row>
     <row r="313" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A313" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B313" t="s">
-        <v>2</v>
+        <v>416</v>
       </c>
     </row>
     <row r="314" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A314" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B314" t="s">
-        <v>2</v>
+        <v>417</v>
       </c>
     </row>
     <row r="315" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A315" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B315" t="s">
-        <v>2</v>
+        <v>418</v>
       </c>
     </row>
     <row r="316" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A316" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B316" t="s">
-        <v>2</v>
+        <v>419</v>
       </c>
     </row>
     <row r="317" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A317" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B317" t="s">
-        <v>2</v>
+        <v>420</v>
       </c>
     </row>
     <row r="318" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A318" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B318" t="s">
-        <v>2</v>
+        <v>421</v>
       </c>
     </row>
     <row r="319" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A319" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B319" t="s">
-        <v>2</v>
+        <v>422</v>
       </c>
     </row>
     <row r="320" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A320" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B320" t="s">
-        <v>2</v>
+        <v>423</v>
       </c>
     </row>
     <row r="321" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A321" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B321" t="s">
-        <v>2</v>
+        <v>424</v>
       </c>
     </row>
     <row r="322" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A322" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B322" t="s">
-        <v>2</v>
+        <v>425</v>
       </c>
     </row>
     <row r="323" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A323" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B323" t="s">
-        <v>2</v>
+        <v>426</v>
       </c>
     </row>
     <row r="324" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A324" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B324" t="s">
-        <v>2</v>
+        <v>427</v>
       </c>
     </row>
     <row r="325" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A325" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B325" t="s">
-        <v>2</v>
+        <v>428</v>
       </c>
     </row>
     <row r="326" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A326" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B326" t="s">
-        <v>2</v>
+        <v>429</v>
       </c>
     </row>
     <row r="327" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A327" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B327" t="s">
-        <v>2</v>
+        <v>430</v>
       </c>
     </row>
     <row r="328" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A328" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B328" t="s">
-        <v>2</v>
+        <v>431</v>
       </c>
     </row>
     <row r="329" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A329" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B329" t="s">
-        <v>2</v>
+        <v>432</v>
       </c>
     </row>
     <row r="330" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A330" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B330" t="s">
-        <v>2</v>
+        <v>433</v>
       </c>
     </row>
     <row r="331" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A331" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B331" t="s">
-        <v>2</v>
+        <v>434</v>
       </c>
     </row>
     <row r="332" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A332" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B332" t="s">
-        <v>2</v>
+        <v>435</v>
       </c>
     </row>
     <row r="333" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A333" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B333" t="s">
-        <v>2</v>
+        <v>436</v>
+      </c>
+    </row>
+    <row r="334" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A334" t="s">
+        <v>437</v>
+      </c>
+      <c r="B334" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="335" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A335" t="s">
+        <v>438</v>
+      </c>
+      <c r="B335" t="s">
+        <v>440</v>
       </c>
     </row>
   </sheetData>

</xml_diff>